<commit_message>
Exempt process from carbon tax
</commit_message>
<xml_diff>
--- a/InputData/ctrl-settings/BEPEfCT/Boolean Exempt Process Emissions From Carbon Tax.xlsx
+++ b/InputData/ctrl-settings/BEPEfCT/Boolean Exempt Process Emissions From Carbon Tax.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeff-nonadmin\CodeRepositories\eps-us\InputData\ctrl-settings\BEPEfCT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\RMI\Colorado\CO_Model\InputData\ctrl-settings\BEPEfCT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF9C5F2A-A137-4E2A-B155-747310D65F82}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D62EDF99-579A-4EDE-8DE0-08C09CB38B47}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3225" yWindow="1140" windowWidth="24090" windowHeight="14880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1230" yWindow="1635" windowWidth="21450" windowHeight="15480" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -440,7 +440,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -502,7 +502,9 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -516,7 +518,7 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
udpated exempt process emissions, remove US target from webapp
</commit_message>
<xml_diff>
--- a/InputData/ctrl-settings/BEPEfCT/Boolean Exempt Process Emissions From Carbon Tax.xlsx
+++ b/InputData/ctrl-settings/BEPEfCT/Boolean Exempt Process Emissions From Carbon Tax.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\RMI\Colorado\CO_Model\InputData\ctrl-settings\BEPEfCT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D62EDF99-579A-4EDE-8DE0-08C09CB38B47}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04255A0E-6217-461B-9D86-B47FFCBE7739}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1230" yWindow="1635" windowWidth="21450" windowHeight="15480" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1515" yWindow="1515" windowWidth="22440" windowHeight="14790" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="BEPEfCT" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -518,7 +518,7 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>